<commit_message>
feat: add year 2025
</commit_message>
<xml_diff>
--- a/TVV.xlsx
+++ b/TVV.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="91">
   <si>
     <t>3607/2016</t>
   </si>
@@ -303,6 +303,9 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>4829/2024</t>
   </si>
 </sst>
 </file>
@@ -311,9 +314,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="0.0000%"/>
+    <numFmt numFmtId="164" formatCode="0.0000%"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,6 +385,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -421,7 +430,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -477,6 +486,9 @@
     <xf numFmtId="44" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -486,9 +498,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hiperlink" xfId="2" builtinId="8"/>
@@ -1110,8 +1122,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A1:AQ46" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
-  <autoFilter ref="A1:AQ46"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A1:AQ47" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
+  <autoFilter ref="A1:AQ47"/>
   <tableColumns count="43">
     <tableColumn id="1" name="Ano" dataDxfId="42"/>
     <tableColumn id="2" name="Decreto" dataDxfId="41"/>
@@ -1438,10 +1450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ46"/>
+  <dimension ref="A1:AQ47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="AQ47" sqref="AQ47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -7152,6 +7164,137 @@
         <v>3.02</v>
       </c>
     </row>
+    <row r="47" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A47" s="37">
+        <v>2025</v>
+      </c>
+      <c r="B47" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" s="39">
+        <v>342.41</v>
+      </c>
+      <c r="D47" s="39">
+        <v>273.95</v>
+      </c>
+      <c r="E47" s="39">
+        <v>205.42</v>
+      </c>
+      <c r="F47" s="39">
+        <v>164.22</v>
+      </c>
+      <c r="G47" s="39">
+        <v>136.91999999999999</v>
+      </c>
+      <c r="H47" s="39">
+        <v>109.6</v>
+      </c>
+      <c r="I47" s="39">
+        <v>95.73</v>
+      </c>
+      <c r="J47" s="39">
+        <v>82.06</v>
+      </c>
+      <c r="K47" s="39">
+        <v>74.459999999999994</v>
+      </c>
+      <c r="L47" s="39">
+        <v>0</v>
+      </c>
+      <c r="M47" s="39">
+        <v>0</v>
+      </c>
+      <c r="N47" s="39">
+        <v>0</v>
+      </c>
+      <c r="O47" s="39">
+        <v>0</v>
+      </c>
+      <c r="P47" s="39">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="39">
+        <v>0</v>
+      </c>
+      <c r="R47" s="39">
+        <v>0</v>
+      </c>
+      <c r="S47" s="39">
+        <v>0</v>
+      </c>
+      <c r="T47" s="39">
+        <v>0</v>
+      </c>
+      <c r="U47" s="39">
+        <v>0</v>
+      </c>
+      <c r="V47" s="39">
+        <v>0</v>
+      </c>
+      <c r="W47" s="39">
+        <v>153.35</v>
+      </c>
+      <c r="X47" s="39">
+        <v>340.81</v>
+      </c>
+      <c r="Y47" s="39">
+        <v>0</v>
+      </c>
+      <c r="Z47" s="39">
+        <v>613.44000000000005</v>
+      </c>
+      <c r="AA47" s="39">
+        <v>851.98</v>
+      </c>
+      <c r="AB47" s="39">
+        <v>1192.82</v>
+      </c>
+      <c r="AC47" s="39">
+        <v>0</v>
+      </c>
+      <c r="AD47" s="39">
+        <v>255.61</v>
+      </c>
+      <c r="AE47" s="39">
+        <v>0</v>
+      </c>
+      <c r="AF47" s="39">
+        <v>562.32000000000005</v>
+      </c>
+      <c r="AG47" s="39">
+        <v>783.82</v>
+      </c>
+      <c r="AH47" s="39">
+        <v>0</v>
+      </c>
+      <c r="AI47" s="39">
+        <v>0</v>
+      </c>
+      <c r="AJ47" s="39">
+        <v>230.02</v>
+      </c>
+      <c r="AK47" s="39">
+        <v>0</v>
+      </c>
+      <c r="AL47" s="39">
+        <v>494.15</v>
+      </c>
+      <c r="AM47" s="39">
+        <v>647.5</v>
+      </c>
+      <c r="AN47" s="39">
+        <v>0</v>
+      </c>
+      <c r="AO47" s="39">
+        <v>0</v>
+      </c>
+      <c r="AP47" s="39">
+        <v>0</v>
+      </c>
+      <c r="AQ47" s="39">
+        <v>3.17</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -7173,20 +7316,20 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="31"/>
+      <c r="B1" s="34"/>
       <c r="C1" s="8"/>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="31"/>
+      <c r="E1" s="34"/>
       <c r="F1" s="8"/>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="31"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
@@ -7380,17 +7523,17 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
@@ -7404,17 +7547,17 @@
       <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="DQUGja0DnPXWQ+h+EKUW5ebZur65T0vwyWmaGyxWbM73GXV+aEIqHEdhNSYtU3fkdJtsoumDnuDZri4V/gXyTQ==" saltValue="s7PCd7LbdlozeCrYi6r4wQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
@@ -7593,31 +7736,31 @@
       <c r="A2">
         <v>1987</v>
       </c>
-      <c r="B2" s="34">
+      <c r="B2" s="31">
         <v>453.19</v>
       </c>
-      <c r="C2" s="34">
+      <c r="C2" s="31">
         <v>362.59</v>
       </c>
-      <c r="D2" s="34">
+      <c r="D2" s="31">
         <v>271.86</v>
       </c>
-      <c r="E2" s="34">
+      <c r="E2" s="31">
         <v>217.33</v>
       </c>
-      <c r="F2" s="34">
+      <c r="F2" s="31">
         <v>181.22</v>
       </c>
-      <c r="G2" s="34">
+      <c r="G2" s="31">
         <v>145.02000000000001</v>
       </c>
-      <c r="H2" s="34">
+      <c r="H2" s="31">
         <v>126.68</v>
       </c>
-      <c r="I2" s="34">
+      <c r="I2" s="31">
         <v>108.6</v>
       </c>
-      <c r="J2" s="34">
+      <c r="J2" s="31">
         <v>90.5</v>
       </c>
       <c r="K2">
@@ -7753,45 +7896,45 @@
       <c r="A3" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="35">
+      <c r="B3" s="32">
         <f>B2/B1</f>
         <v>1.6086539826778359</v>
       </c>
-      <c r="C3" s="35">
+      <c r="C3" s="32">
         <f t="shared" ref="C3:J3" si="1">C2/C1</f>
         <v>1.608651286601597</v>
       </c>
-      <c r="D3" s="35">
+      <c r="D3" s="32">
         <f t="shared" si="1"/>
         <v>1.6086390532544379</v>
       </c>
-      <c r="E3" s="35">
+      <c r="E3" s="32">
         <f t="shared" si="1"/>
         <v>1.6086602516654331</v>
       </c>
-      <c r="F3" s="35">
+      <c r="F3" s="32">
         <f t="shared" si="1"/>
         <v>1.6086995117620948</v>
       </c>
-      <c r="G3" s="35">
+      <c r="G3" s="32">
         <f t="shared" si="1"/>
         <v>1.6086522462562396</v>
       </c>
-      <c r="H3" s="35">
+      <c r="H3" s="32">
         <f t="shared" si="1"/>
         <v>1.6086349206349206</v>
       </c>
-      <c r="I3" s="35">
+      <c r="I3" s="32">
         <f t="shared" si="1"/>
         <v>1.6086505702858833</v>
       </c>
-      <c r="J3" s="35">
+      <c r="J3" s="32">
         <f t="shared" si="1"/>
         <v>1.6086029150373267</v>
       </c>
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A4" s="36">
+      <c r="A4" s="33">
         <f>AVERAGE(B3:J3)</f>
         <v>1.6086494153528634</v>
       </c>

</xml_diff>